<commit_message>
do a little extra 👾
</commit_message>
<xml_diff>
--- a/table_keys.xlsx
+++ b/table_keys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GM\Documents\local_dev\help-me-convert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FE50AB-F0CC-4951-9C3A-595DA4EA8825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD422F6-6004-46D6-B435-6811499A3A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{33BE4143-853D-43C6-A07A-1AD569C2E022}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{33BE4143-853D-43C6-A07A-1AD569C2E022}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8020" uniqueCount="2419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8020" uniqueCount="2420">
   <si>
     <t>sourceTable</t>
   </si>
@@ -7319,6 +7319,9 @@
   </si>
   <si>
     <t>werks, charg, sap_hold, src_hold, mandt, lgort, matnr</t>
+  </si>
+  <si>
+    <t>table_keys</t>
   </si>
 </sst>
 </file>
@@ -7703,7 +7706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA31F2A5-9BC0-4A1F-975C-C7E7483D47E0}">
   <dimension ref="A1:E3158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A838" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R855" sqref="R855"/>
     </sheetView>
   </sheetViews>
@@ -38949,8 +38952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4017ABF0-FD74-4007-8025-B918CA5996E0}">
   <dimension ref="A1:B851"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38964,7 +38967,7 @@
         <v>1611</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1612</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -45773,12 +45776,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45953,15 +45953,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69065D09-7C20-4429-BC31-BE1747F7E6BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE6A5F3F-8105-4FD2-99CB-852EF5E6722A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45986,10 +45990,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE6A5F3F-8105-4FD2-99CB-852EF5E6722A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69065D09-7C20-4429-BC31-BE1747F7E6BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>